<commit_message>
Update email address in Excel template
</commit_message>
<xml_diff>
--- a/data/ihcc-data-dictionary-registration-template.xlsx
+++ b/data/ihcc-data-dictionary-registration-template.xlsx
@@ -24,7 +24,7 @@
     <t>Email to</t>
   </si>
   <si>
-    <t>james@overton.ca</t>
+    <t>ihcc-browser@googlegroups.com</t>
   </si>
   <si>
     <t>Metadata</t>
@@ -106,7 +106,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -114,6 +114,8 @@
     </font>
     <font>
       <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color theme="1"/>
@@ -123,7 +125,6 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -139,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -152,10 +153,7 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
@@ -418,7 +416,7 @@
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -429,7 +427,7 @@
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -440,7 +438,7 @@
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -451,7 +449,7 @@
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -459,10 +457,10 @@
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -475,7 +473,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -486,7 +484,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -497,7 +495,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -508,18 +506,18 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -552,27 +550,27 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" ht="33.75" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" ht="33.0" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -601,19 +599,19 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add all metadata elements to registration
</commit_message>
<xml_diff>
--- a/data/ihcc-data-dictionary-registration-template.xlsx
+++ b/data/ihcc-data-dictionary-registration-template.xlsx
@@ -1,19 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tauber/github/IHCC/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914C5192-75C9-DB4B-9000-53C90E08C140}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-37020" yWindow="860" windowWidth="33600" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Instructions" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Metadata" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Terminology" sheetId="3" r:id="rId6"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" r:id="rId2"/>
+    <sheet name="Terminology" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
   <si>
     <t>IHCC Data Harmonization</t>
   </si>
@@ -39,9 +48,6 @@
     <t>The short identifier for the cohort. Must be one word, uppercase, and unique among the IHCC cohorts</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>The title of the cohort.</t>
   </si>
   <si>
@@ -81,9 +87,6 @@
     <t>Parent Term</t>
   </si>
   <si>
-    <t>The parent term: this is optional, but if filled the value must be the label of another term.</t>
-  </si>
-  <si>
     <t>Definition</t>
   </si>
   <si>
@@ -100,86 +103,249 @@
   </si>
   <si>
     <t>Other comments for the IHCC data harmonization team.</t>
+  </si>
+  <si>
+    <t>PI/Lead</t>
+  </si>
+  <si>
+    <t>Enrollment Start Year</t>
+  </si>
+  <si>
+    <t>Enrollment End Year</t>
+  </si>
+  <si>
+    <t>Total Enrollment</t>
+  </si>
+  <si>
+    <t>Target Enrollment</t>
+  </si>
+  <si>
+    <t>Available Datatypes</t>
+  </si>
+  <si>
+    <t>Enrollment</t>
+  </si>
+  <si>
+    <t>Biospecimens</t>
+  </si>
+  <si>
+    <t>Environmental Data</t>
+  </si>
+  <si>
+    <t>Genomic Data</t>
+  </si>
+  <si>
+    <t>Phenotypic Data</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Identifiers</t>
+  </si>
+  <si>
+    <t>Cohort Name</t>
+  </si>
+  <si>
+    <t>Please select TRUE or FALSE</t>
+  </si>
+  <si>
+    <t>Enrollment Data</t>
+  </si>
+  <si>
+    <t>Required*</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE values for the types of data collected by the cohort.</t>
+  </si>
+  <si>
+    <t>Enrollment years and numbers for the cohort. Enrollment start year and total enrollment values are required, other values are optional.</t>
+  </si>
+  <si>
+    <t>The cohort PI/Lead (comma-separated for more than one lead).</t>
+  </si>
+  <si>
+    <t>A link to the cohort website.</t>
+  </si>
+  <si>
+    <t>The parent term or category: this is optional, but if filled, the value must be the label of another term in this sheet.</t>
+  </si>
+  <si>
+    <t>Data Sharing</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE value for if the cohort has IRB approval for data sharing.</t>
+  </si>
+  <si>
+    <t>Countries</t>
+  </si>
+  <si>
+    <t>Country(ies) in which the cohort participants are located (comma-separated).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -369,34 +535,38 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="12.0"/>
-    <col customWidth="1" min="3" max="3" width="38.71"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" ht="53" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -404,12 +574,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -420,202 +590,416 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="2" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="s">
+      <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="2" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="s">
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="2" t="s">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B3"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.29"/>
-    <col customWidth="1" min="2" max="2" width="50.14"/>
+    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" ht="33.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" ht="33.0" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="B2" s="14"/>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="14"/>
+    </row>
+    <row r="4" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A4" s="5"/>
+    </row>
+    <row r="5" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11"/>
+    </row>
+    <row r="6" spans="1:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="14"/>
+    </row>
+    <row r="8" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="14"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="14"/>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="14"/>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
+      <c r="B13" s="14"/>
+    </row>
+    <row r="14" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="11"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="14"/>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="14"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="14"/>
+    </row>
+    <row r="20" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="14"/>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="14"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="14"/>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="14"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <dataValidations count="14">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enrollment start year must be between 1900 and 2021. If your enrollment start year falls outside this range, ignore this message." promptTitle="Enrollment Start Year (required)" prompt="Please enter a year" sqref="B15" xr:uid="{80AEF0CD-843B-E048-805D-AE0368B89C43}">
+      <formula1>1900</formula1>
+      <formula2>2021</formula2>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Year should be between 1900 and 2050. If your enrollment end year falls outside this range, ignore this message." promptTitle="Enrollment End Year (optional)" prompt="Please enter a year. Leave blank if enrollment is ongoing." sqref="B16" xr:uid="{C8D56C3F-A455-034B-BF75-16978927B2D5}">
+      <formula1>1900</formula1>
+      <formula2>2050</formula2>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="information" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The total enrollment must be a number greater than zero." promptTitle="Total Enrollment (required)" prompt="Please enter the number of participants enrolled in this cohort." sqref="B17" xr:uid="{54488446-FC1C-1A43-A6CA-CF221C469A55}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="information" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The target enrollment must be a number greater than zero. Leave blank if you do not have a target enrollment." promptTitle="Target Enrollment (optional)" prompt="Please enter the target enrollment for this cohort. Leave blank if you do not have a target enrollment." sqref="B18" xr:uid="{5A37B875-23D0-1C40-BB08-3CBAAA8513E5}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21:B24" xr:uid="{919B4EB2-315E-6640-A0BB-B4BD7F718E4B}">
+      <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Regions (required)" prompt="Please enter the region(s) in which this cohort's participants are located. For mulitple regions, please enter a comma-separated list." sqref="B11" xr:uid="{A7DCFCAD-FFC0-3145-BF3B-A9899795C60F}"/>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" error="Please make sure your cohort ID is all uppercase and does not contain spaces." promptTitle="Cohort ID (required)" prompt="Select a one-word, uppercase identifier for your cohort." sqref="B2" xr:uid="{8118F1D8-3BE7-CF40-B377-43FE9C72F7BB}">
+      <formula1>AND(EXACT(B2,UPPER(B2)), ISERROR(FIND(" ",B2)))</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description (required)" prompt="Please enter a short text description (one to two sentences) describing your cohort." sqref="B6" xr:uid="{B2EE65F5-3B16-894A-BEEC-FFCE8C0B4AFA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Cohort Name (required)" prompt="Please enter the full name/title of your cohort." sqref="B3" xr:uid="{2D54D473-1D07-F24D-A03D-FC7AEA2E2CE4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="License (required)" prompt="Please enter a link to your license (e.g., https://creativecommons.org/licenses/by/4.0/)" sqref="B7" xr:uid="{1DB3E865-F786-5E45-A2A6-952E6FAA7235}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Rights (optional)" prompt="Please enter a short text description of the usage rights for your cohort's data dictionary." sqref="B8" xr:uid="{8CD8A150-C679-854F-A0C5-D31BA0B59FC6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Website (optional)" prompt="Please enter the link to your cohort's website." sqref="B9" xr:uid="{2BC9BB7B-AFCF-2E41-BE80-5BB52653DEE3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="PI/Lead (required)" prompt="Please enter the PI lead or leads. If multiple leads, please make sure the names are comma-separated." sqref="B10" xr:uid="{616AC0FD-6AB5-D442-BF08-672C6CD3A66C}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Sharing (required)" prompt="Please select TRUE or FALSE if your cohort has IRB approval for data sharing." sqref="B12" xr:uid="{C866797D-F558-EB48-9C22-4F0CA8C52C4F}">
+      <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.71"/>
-    <col customWidth="1" min="2" max="2" width="17.86"/>
-    <col customWidth="1" min="3" max="4" width="26.0"/>
-    <col customWidth="1" min="5" max="5" width="28.0"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>27</v>
-      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix datatypes and phenotypic data
</commit_message>
<xml_diff>
--- a/data/ihcc-data-dictionary-registration-template.xlsx
+++ b/data/ihcc-data-dictionary-registration-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tauber/github/IHCC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914C5192-75C9-DB4B-9000-53C90E08C140}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42844E6C-99B3-C547-BFAB-73683A8072BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37020" yWindow="860" windowWidth="33600" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,9 +135,6 @@
     <t>Genomic Data</t>
   </si>
   <si>
-    <t>Phenotypic Data</t>
-  </si>
-  <si>
     <t>Website</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>Country(ies) in which the cohort participants are located (comma-separated).</t>
+  </si>
+  <si>
+    <t>Phenotypic/Clinical Data</t>
   </si>
 </sst>
 </file>
@@ -198,17 +198,20 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -320,18 +323,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -592,7 +584,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
@@ -636,13 +628,13 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -653,40 +645,40 @@
         <v>6</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>43</v>
-      </c>
       <c r="C15" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -697,7 +689,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -731,7 +723,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -792,7 +784,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="11"/>
     </row>
@@ -804,7 +796,7 @@
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="14"/>
     </row>
@@ -837,7 +829,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="14"/>
     </row>
@@ -849,13 +841,13 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="14"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="14"/>
     </row>
@@ -898,7 +890,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -921,7 +913,7 @@
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B24" s="14"/>
     </row>

</xml_diff>

<commit_message>
Add all metadata elements to registration (#144)
* Add all metadata elements to registration

* Fix datatypes and phenotypic data

* Add script to convert metadata to CSV

* Fix test prefix
</commit_message>
<xml_diff>
--- a/data/ihcc-data-dictionary-registration-template.xlsx
+++ b/data/ihcc-data-dictionary-registration-template.xlsx
@@ -1,19 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tauber/github/IHCC/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42844E6C-99B3-C547-BFAB-73683A8072BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-37020" yWindow="860" windowWidth="33600" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Instructions" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Metadata" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Terminology" sheetId="3" r:id="rId6"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" r:id="rId2"/>
+    <sheet name="Terminology" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
   <si>
     <t>IHCC Data Harmonization</t>
   </si>
@@ -39,9 +48,6 @@
     <t>The short identifier for the cohort. Must be one word, uppercase, and unique among the IHCC cohorts</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>The title of the cohort.</t>
   </si>
   <si>
@@ -81,9 +87,6 @@
     <t>Parent Term</t>
   </si>
   <si>
-    <t>The parent term: this is optional, but if filled the value must be the label of another term.</t>
-  </si>
-  <si>
     <t>Definition</t>
   </si>
   <si>
@@ -100,86 +103,241 @@
   </si>
   <si>
     <t>Other comments for the IHCC data harmonization team.</t>
+  </si>
+  <si>
+    <t>PI/Lead</t>
+  </si>
+  <si>
+    <t>Enrollment Start Year</t>
+  </si>
+  <si>
+    <t>Enrollment End Year</t>
+  </si>
+  <si>
+    <t>Total Enrollment</t>
+  </si>
+  <si>
+    <t>Target Enrollment</t>
+  </si>
+  <si>
+    <t>Available Datatypes</t>
+  </si>
+  <si>
+    <t>Enrollment</t>
+  </si>
+  <si>
+    <t>Biospecimens</t>
+  </si>
+  <si>
+    <t>Environmental Data</t>
+  </si>
+  <si>
+    <t>Genomic Data</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Identifiers</t>
+  </si>
+  <si>
+    <t>Cohort Name</t>
+  </si>
+  <si>
+    <t>Please select TRUE or FALSE</t>
+  </si>
+  <si>
+    <t>Enrollment Data</t>
+  </si>
+  <si>
+    <t>Required*</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE values for the types of data collected by the cohort.</t>
+  </si>
+  <si>
+    <t>Enrollment years and numbers for the cohort. Enrollment start year and total enrollment values are required, other values are optional.</t>
+  </si>
+  <si>
+    <t>The cohort PI/Lead (comma-separated for more than one lead).</t>
+  </si>
+  <si>
+    <t>A link to the cohort website.</t>
+  </si>
+  <si>
+    <t>The parent term or category: this is optional, but if filled, the value must be the label of another term in this sheet.</t>
+  </si>
+  <si>
+    <t>Data Sharing</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE value for if the cohort has IRB approval for data sharing.</t>
+  </si>
+  <si>
+    <t>Countries</t>
+  </si>
+  <si>
+    <t>Country(ies) in which the cohort participants are located (comma-separated).</t>
+  </si>
+  <si>
+    <t>Phenotypic/Clinical Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -369,34 +527,38 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="12.0"/>
-    <col customWidth="1" min="3" max="3" width="38.71"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" ht="53" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -404,12 +566,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -420,202 +582,416 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="2" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="s">
+      <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="2" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="s">
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="2" t="s">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B3"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.29"/>
-    <col customWidth="1" min="2" max="2" width="50.14"/>
+    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" ht="33.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" ht="33.0" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="B2" s="14"/>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="14"/>
+    </row>
+    <row r="4" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A4" s="5"/>
+    </row>
+    <row r="5" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11"/>
+    </row>
+    <row r="6" spans="1:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="14"/>
+    </row>
+    <row r="8" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="14"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="14"/>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="14"/>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
+      <c r="B13" s="14"/>
+    </row>
+    <row r="14" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="11"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="14"/>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="14"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="14"/>
+    </row>
+    <row r="20" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="14"/>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="14"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="14"/>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="14"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <dataValidations count="14">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enrollment start year must be between 1900 and 2021. If your enrollment start year falls outside this range, ignore this message." promptTitle="Enrollment Start Year (required)" prompt="Please enter a year" sqref="B15" xr:uid="{80AEF0CD-843B-E048-805D-AE0368B89C43}">
+      <formula1>1900</formula1>
+      <formula2>2021</formula2>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Year should be between 1900 and 2050. If your enrollment end year falls outside this range, ignore this message." promptTitle="Enrollment End Year (optional)" prompt="Please enter a year. Leave blank if enrollment is ongoing." sqref="B16" xr:uid="{C8D56C3F-A455-034B-BF75-16978927B2D5}">
+      <formula1>1900</formula1>
+      <formula2>2050</formula2>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="information" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The total enrollment must be a number greater than zero." promptTitle="Total Enrollment (required)" prompt="Please enter the number of participants enrolled in this cohort." sqref="B17" xr:uid="{54488446-FC1C-1A43-A6CA-CF221C469A55}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="information" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The target enrollment must be a number greater than zero. Leave blank if you do not have a target enrollment." promptTitle="Target Enrollment (optional)" prompt="Please enter the target enrollment for this cohort. Leave blank if you do not have a target enrollment." sqref="B18" xr:uid="{5A37B875-23D0-1C40-BB08-3CBAAA8513E5}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21:B24" xr:uid="{919B4EB2-315E-6640-A0BB-B4BD7F718E4B}">
+      <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Regions (required)" prompt="Please enter the region(s) in which this cohort's participants are located. For mulitple regions, please enter a comma-separated list." sqref="B11" xr:uid="{A7DCFCAD-FFC0-3145-BF3B-A9899795C60F}"/>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" error="Please make sure your cohort ID is all uppercase and does not contain spaces." promptTitle="Cohort ID (required)" prompt="Select a one-word, uppercase identifier for your cohort." sqref="B2" xr:uid="{8118F1D8-3BE7-CF40-B377-43FE9C72F7BB}">
+      <formula1>AND(EXACT(B2,UPPER(B2)), ISERROR(FIND(" ",B2)))</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description (required)" prompt="Please enter a short text description (one to two sentences) describing your cohort." sqref="B6" xr:uid="{B2EE65F5-3B16-894A-BEEC-FFCE8C0B4AFA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Cohort Name (required)" prompt="Please enter the full name/title of your cohort." sqref="B3" xr:uid="{2D54D473-1D07-F24D-A03D-FC7AEA2E2CE4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="License (required)" prompt="Please enter a link to your license (e.g., https://creativecommons.org/licenses/by/4.0/)" sqref="B7" xr:uid="{1DB3E865-F786-5E45-A2A6-952E6FAA7235}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Rights (optional)" prompt="Please enter a short text description of the usage rights for your cohort's data dictionary." sqref="B8" xr:uid="{8CD8A150-C679-854F-A0C5-D31BA0B59FC6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Website (optional)" prompt="Please enter the link to your cohort's website." sqref="B9" xr:uid="{2BC9BB7B-AFCF-2E41-BE80-5BB52653DEE3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="PI/Lead (required)" prompt="Please enter the PI lead or leads. If multiple leads, please make sure the names are comma-separated." sqref="B10" xr:uid="{616AC0FD-6AB5-D442-BF08-672C6CD3A66C}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Sharing (required)" prompt="Please select TRUE or FALSE if your cohort has IRB approval for data sharing." sqref="B12" xr:uid="{C866797D-F558-EB48-9C22-4F0CA8C52C4F}">
+      <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.71"/>
-    <col customWidth="1" min="2" max="2" width="17.86"/>
-    <col customWidth="1" min="3" max="4" width="26.0"/>
-    <col customWidth="1" min="5" max="5" width="28.0"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>27</v>
-      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add collected imaging variables and polygenic risk scores
</commit_message>
<xml_diff>
--- a/data/ihcc-data-dictionary-registration-template.xlsx
+++ b/data/ihcc-data-dictionary-registration-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tauber/github/IHCC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A7EEB88-D2BB-3C4C-B400-8ECEE106E378}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B28D489-23E9-3B4B-9ECF-2E407850626C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37020" yWindow="860" windowWidth="33600" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
   <si>
     <t>IHCC Data Harmonization</t>
   </si>
@@ -196,6 +196,27 @@
   </si>
   <si>
     <t>Enrollment years and numbers for the cohort. Enrollment end year and target enrollment are optional.</t>
+  </si>
+  <si>
+    <t>Collected Imaging</t>
+  </si>
+  <si>
+    <t>MRI</t>
+  </si>
+  <si>
+    <t>PET</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE values for the types of imaging collected by the cohort.</t>
+  </si>
+  <si>
+    <t>Polygenic Risk Scores</t>
   </si>
 </sst>
 </file>
@@ -349,10 +370,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -556,7 +573,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -712,69 +729,80 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
+      <c r="A17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>45</v>
+        <v>6</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>22</v>
+      <c r="C21" s="17" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
+      <c r="A22" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="4" t="s">
-        <v>25</v>
+      <c r="A23" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -791,7 +819,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -965,6 +993,44 @@
         <v>50</v>
       </c>
       <c r="B29" s="14"/>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="14"/>
+    </row>
+    <row r="32" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="14"/>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="14"/>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="14"/>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="14"/>
     </row>
   </sheetData>
   <dataValidations count="17">
@@ -982,7 +1048,7 @@
     <dataValidation type="whole" errorStyle="information" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The target enrollment must be a number greater than zero. Leave blank if you do not have a target enrollment." promptTitle="Target Enrollment (optional)" prompt="Please enter the target enrollment for this cohort. Leave blank if you do not have a target enrollment." sqref="B18" xr:uid="{5A37B875-23D0-1C40-BB08-3CBAAA8513E5}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:B29" xr:uid="{919B4EB2-315E-6640-A0BB-B4BD7F718E4B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:B30 B33:B36" xr:uid="{919B4EB2-315E-6640-A0BB-B4BD7F718E4B}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Regions (required)" prompt="Please enter the region(s) in which this cohort's participants are located. For mulitple regions, please enter a comma-separated list." sqref="B11" xr:uid="{A7DCFCAD-FFC0-3145-BF3B-A9899795C60F}"/>

</xml_diff>